<commit_message>
Make permeabilization time value and unit as optional
</commit_message>
<xml_diff>
--- a/visium/latest/visium.xlsx
+++ b/visium/latest/visium.xlsx
@@ -131,12 +131,12 @@
     </comment>
     <comment ref="O1" authorId="1">
       <text>
-        <t>(Required) Permeabilization time used for this tissue section.</t>
+        <t>Permeabilization time used for this tissue section.</t>
       </text>
     </comment>
     <comment ref="P1" authorId="1">
       <text>
-        <t>(Required) The unit for the permeabilization time.</t>
+        <t>The unit for the permeabilization time.</t>
       </text>
     </comment>
     <comment ref="Q1" authorId="1">
@@ -531,7 +531,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-10-09T19:11:54-07:00</t>
+    <t>2023-10-16T20:50:31-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>

</xml_diff>

<commit_message>
Remove probes from Visium
</commit_message>
<xml_diff>
--- a/visium/latest/visium.xlsx
+++ b/visium/latest/visium.xlsx
@@ -13,8 +13,7 @@
     <sheet name="spot_spacing_unit" r:id="rId7" sheetId="5"/>
     <sheet name="capture_area_id" r:id="rId8" sheetId="6"/>
     <sheet name="permeabilization_time_unit" r:id="rId9" sheetId="7"/>
-    <sheet name="rna_probe_panel" r:id="rId10" sheetId="8"/>
-    <sheet name=".metadata" r:id="rId11" sheetId="9"/>
+    <sheet name=".metadata" r:id="rId10" sheetId="8"/>
   </sheets>
 </workbook>
 </file>
@@ -141,18 +140,6 @@
     </comment>
     <comment ref="Q1" authorId="1">
       <text>
-        <t>(Required) This is the probe panel used to target genes. If a custom panel is
-used, then the list of target gene needs to be uploaded with the dataset files.</t>
-      </text>
-    </comment>
-    <comment ref="R1" authorId="1">
-      <text>
-        <t>State ("Yes" or "No") whether custom RNA or antibody probes were used. If custom
-probes are used, a file including the panel components must be included.</t>
-      </text>
-    </comment>
-    <comment ref="S1" authorId="1">
-      <text>
         <t>(Required) The string that serves as the definitive identifier for the metadata
 schema version and is readily interpretable by computers for data validation and
 processing. Example: 22bc762a-5020-419d-b170-24253ed9e8d9</t>
@@ -163,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="117">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -195,6 +182,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000246</t>
   </si>
   <si>
+    <t>MIBI</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000172</t>
+  </si>
+  <si>
     <t>DESI</t>
   </si>
   <si>
@@ -255,12 +248,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000222</t>
   </si>
   <si>
-    <t>Multiplex Ion Beam Imaging</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000172</t>
-  </si>
-  <si>
     <t>SIMS</t>
   </si>
   <si>
@@ -489,30 +476,6 @@
     <t>http://purl.obolibrary.org/obo/UO_0000031</t>
   </si>
   <si>
-    <t>rna_probe_panel</t>
-  </si>
-  <si>
-    <t>Custom</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C126386</t>
-  </si>
-  <si>
-    <t>Not applicable</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C48660</t>
-  </si>
-  <si>
-    <t>10x Genomics; Visium Human Transcriptome Probe Kit v2 - Small; PN 1000466</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000274</t>
-  </si>
-  <si>
-    <t>is_custom_probes_used</t>
-  </si>
-  <si>
     <t>metadata_schema_id</t>
   </si>
   <si>
@@ -531,7 +494,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-10-16T20:50:31-07:00</t>
+    <t>2023-10-20T15:02:19-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -590,7 +553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyAlignment="true" applyFill="true">
       <alignment horizontal="center"/>
@@ -612,8 +575,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -624,7 +585,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -646,9 +607,7 @@
     <col min="14" max="14" style="15" width="15.05859375" customWidth="true" bestFit="true"/>
     <col min="15" max="15" style="16" width="26.43359375" customWidth="true" bestFit="true"/>
     <col min="16" max="16" style="17" width="25.2734375" customWidth="true" bestFit="true"/>
-    <col min="17" max="17" style="18" width="15.83984375" customWidth="true" bestFit="true"/>
-    <col min="18" max="18" style="19" width="22.1796875" customWidth="true" bestFit="true"/>
-    <col min="19" max="19" style="20" width="19.61328125" customWidth="true" bestFit="true"/>
+    <col min="17" max="17" style="18" width="19.61328125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -703,20 +662,14 @@
       <c r="Q1" t="s" s="1">
         <v>108</v>
       </c>
-      <c r="R1" t="s" s="1">
-        <v>115</v>
-      </c>
-      <c r="S1" t="s" s="1">
-        <v>116</v>
-      </c>
     </row>
     <row r="2">
-      <c r="S2" t="s">
-        <v>117</v>
+      <c r="Q2" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="12">
+  <dataValidations count="11">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'dataset_type'!$A$1:$A$36</formula1>
     </dataValidation>
@@ -755,9 +708,6 @@
     <dataValidation type="list" sqref="P2:P1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'permeabilization_time_unit'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="Q2:Q1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'rna_probe_panel'!$A$1:$A$3</formula1>
-    </dataValidation>
   </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing r:id="rId1"/>
@@ -1241,43 +1191,6 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1292,16 +1205,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B1" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2">
@@ -1309,13 +1222,13 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Visium with new preparation instrument vendor and model fields
</commit_message>
<xml_diff>
--- a/visium/latest/visium.xlsx
+++ b/visium/latest/visium.xlsx
@@ -13,7 +13,9 @@
     <sheet name="spot_spacing_unit" r:id="rId7" sheetId="5"/>
     <sheet name="capture_area_id" r:id="rId8" sheetId="6"/>
     <sheet name="permeabilization_time_unit" r:id="rId9" sheetId="7"/>
-    <sheet name=".metadata" r:id="rId10" sheetId="8"/>
+    <sheet name="preparation_instrument_vendor" r:id="rId10" sheetId="8"/>
+    <sheet name="preparation_instrument_model" r:id="rId11" sheetId="9"/>
+    <sheet name=".metadata" r:id="rId12" sheetId="10"/>
   </sheets>
 </workbook>
 </file>
@@ -141,6 +143,21 @@
     </comment>
     <comment ref="Q1" authorId="1">
       <text>
+        <t>(Required) The manufacturer of the instrument used to prepare
+(staining/processing) the sample for the assay. If an automatic slide staining
+method was indicated this field should list the manufacturer of the instrument.</t>
+      </text>
+    </comment>
+    <comment ref="R1" authorId="1">
+      <text>
+        <t>(Required) Manufacturers of a staining system instrument may offer various
+versions (models) of that instrument with different features. Differences in
+features or sensitivities may be relevant to processing or interpretation of the
+data.</t>
+      </text>
+    </comment>
+    <comment ref="S1" authorId="1">
+      <text>
         <t>(Required) The string that serves as the definitive identifier for the metadata
 schema version and is readily interpretable by computers for data validation and
 processing. Example: 22bc762a-5020-419d-b170-24253ed9e8d9</t>
@@ -151,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="159">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -477,6 +494,132 @@
     <t>http://purl.obolibrary.org/obo/UO_0000031</t>
   </si>
   <si>
+    <t>preparation_instrument_vendor</t>
+  </si>
+  <si>
+    <t>In-House</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C126386</t>
+  </si>
+  <si>
+    <t>Leica Biosystems</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023603</t>
+  </si>
+  <si>
+    <t>Not applicable</t>
+  </si>
+  <si>
+    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C48660</t>
+  </si>
+  <si>
+    <t>HTX Technologies</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023734</t>
+  </si>
+  <si>
+    <t>10x Genomics</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023672</t>
+  </si>
+  <si>
+    <t>Hamamatsu</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_017105</t>
+  </si>
+  <si>
+    <t>SunChrom</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023908</t>
+  </si>
+  <si>
+    <t>preparation_instrument_model</t>
+  </si>
+  <si>
+    <t>NanoZoomer S210</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023760</t>
+  </si>
+  <si>
+    <t>Sublimator</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023729</t>
+  </si>
+  <si>
+    <t>Chromium Controller</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_019326</t>
+  </si>
+  <si>
+    <t>NanoZoomer S360</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023761</t>
+  </si>
+  <si>
+    <t>NanoZoomer S60</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023762</t>
+  </si>
+  <si>
+    <t>Chromium X</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024537</t>
+  </si>
+  <si>
+    <t>AutoStainer XL</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023957</t>
+  </si>
+  <si>
+    <t>Visium CytAssist</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024570</t>
+  </si>
+  <si>
+    <t>SunCollect Sprayer</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023907</t>
+  </si>
+  <si>
+    <t>M3+ Sprayer</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023731</t>
+  </si>
+  <si>
+    <t>Chromium iX</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024536</t>
+  </si>
+  <si>
+    <t>M5 Sprayer</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023733</t>
+  </si>
+  <si>
+    <t>TM-Sprayer</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023732</t>
+  </si>
+  <si>
     <t>metadata_schema_id</t>
   </si>
   <si>
@@ -495,7 +638,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-10-27T18:09:16-07:00</t>
+    <t>2023-11-01T13:54:36-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -554,7 +697,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyAlignment="true" applyFill="true">
       <alignment horizontal="center"/>
@@ -576,6 +719,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -586,7 +731,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -608,7 +753,9 @@
     <col min="14" max="14" style="15" width="15.05859375" customWidth="true" bestFit="true"/>
     <col min="15" max="15" style="16" width="26.43359375" customWidth="true" bestFit="true"/>
     <col min="16" max="16" style="17" width="25.2734375" customWidth="true" bestFit="true"/>
-    <col min="17" max="17" style="18" width="19.61328125" customWidth="true" bestFit="true"/>
+    <col min="17" max="17" style="18" width="29.08203125" customWidth="true" bestFit="true"/>
+    <col min="18" max="18" style="19" width="28.48828125" customWidth="true" bestFit="true"/>
+    <col min="19" max="19" style="20" width="19.61328125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -663,14 +810,20 @@
       <c r="Q1" t="s" s="1">
         <v>108</v>
       </c>
+      <c r="R1" t="s" s="1">
+        <v>123</v>
+      </c>
+      <c r="S1" t="s" s="1">
+        <v>150</v>
+      </c>
     </row>
     <row r="2">
-      <c r="Q2" t="s">
-        <v>109</v>
+      <c r="S2" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="11">
+  <dataValidations count="13">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'dataset_type'!$A$1:$A$36</formula1>
     </dataValidation>
@@ -709,10 +862,63 @@
     <dataValidation type="list" sqref="P2:P1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'permeabilization_time_unit'!$A$1:$A$1</formula1>
     </dataValidation>
+    <dataValidation type="list" sqref="Q2:Q1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+      <formula1>'preparation_instrument_vendor'!$A$1:$A$7</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="R2:R1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+      <formula1>'preparation_instrument_model'!$A$1:$A$14</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.1875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="27.9921875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="80.6640625" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -1192,44 +1398,191 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="11.83203125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.1875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="27.9921875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="80.6640625" customWidth="true" bestFit="true"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" t="s">
         <v>110</v>
-      </c>
-      <c r="B1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
         <v>112</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" t="s">
         <v>114</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" t="s">
         <v>116</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B11" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>146</v>
+      </c>
+      <c r="B13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Roll back changes on Visium
</commit_message>
<xml_diff>
--- a/visium/latest/visium.xlsx
+++ b/visium/latest/visium.xlsx
@@ -13,9 +13,7 @@
     <sheet name="spot_spacing_unit" r:id="rId7" sheetId="5"/>
     <sheet name="capture_area_id" r:id="rId8" sheetId="6"/>
     <sheet name="permeabilization_time_unit" r:id="rId9" sheetId="7"/>
-    <sheet name="preparation_instrument_vendor" r:id="rId10" sheetId="8"/>
-    <sheet name="preparation_instrument_model" r:id="rId11" sheetId="9"/>
-    <sheet name=".metadata" r:id="rId12" sheetId="10"/>
+    <sheet name=".metadata" r:id="rId10" sheetId="8"/>
   </sheets>
 </workbook>
 </file>
@@ -143,21 +141,6 @@
     </comment>
     <comment ref="Q1" authorId="1">
       <text>
-        <t>(Required) The manufacturer of the instrument used to prepare
-(staining/processing) the sample for the assay. If an automatic slide staining
-method was indicated this field should list the manufacturer of the instrument.</t>
-      </text>
-    </comment>
-    <comment ref="R1" authorId="1">
-      <text>
-        <t>(Required) Manufacturers of a staining system instrument may offer various
-versions (models) of that instrument with different features. Differences in
-features or sensitivities may be relevant to processing or interpretation of the
-data.</t>
-      </text>
-    </comment>
-    <comment ref="S1" authorId="1">
-      <text>
         <t>(Required) The string that serves as the definitive identifier for the metadata
 schema version and is readily interpretable by computers for data validation and
 processing. Example: 22bc762a-5020-419d-b170-24253ed9e8d9</t>
@@ -168,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="117">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -494,132 +477,6 @@
     <t>http://purl.obolibrary.org/obo/UO_0000031</t>
   </si>
   <si>
-    <t>preparation_instrument_vendor</t>
-  </si>
-  <si>
-    <t>In-House</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C126386</t>
-  </si>
-  <si>
-    <t>Leica Biosystems</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023603</t>
-  </si>
-  <si>
-    <t>Not applicable</t>
-  </si>
-  <si>
-    <t>http://ncicb.nci.nih.gov/xml/owl/EVS/Thesaurus.owl#C48660</t>
-  </si>
-  <si>
-    <t>HTX Technologies</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023734</t>
-  </si>
-  <si>
-    <t>10x Genomics</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023672</t>
-  </si>
-  <si>
-    <t>Hamamatsu</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_017105</t>
-  </si>
-  <si>
-    <t>SunChrom</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023908</t>
-  </si>
-  <si>
-    <t>preparation_instrument_model</t>
-  </si>
-  <si>
-    <t>NanoZoomer S210</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023760</t>
-  </si>
-  <si>
-    <t>Sublimator</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023729</t>
-  </si>
-  <si>
-    <t>Chromium Controller</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_019326</t>
-  </si>
-  <si>
-    <t>NanoZoomer S360</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023761</t>
-  </si>
-  <si>
-    <t>NanoZoomer S60</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023762</t>
-  </si>
-  <si>
-    <t>Chromium X</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024537</t>
-  </si>
-  <si>
-    <t>AutoStainer XL</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023957</t>
-  </si>
-  <si>
-    <t>Visium CytAssist</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024570</t>
-  </si>
-  <si>
-    <t>SunCollect Sprayer</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023907</t>
-  </si>
-  <si>
-    <t>M3+ Sprayer</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023731</t>
-  </si>
-  <si>
-    <t>Chromium iX</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_024536</t>
-  </si>
-  <si>
-    <t>M5 Sprayer</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023733</t>
-  </si>
-  <si>
-    <t>TM-Sprayer</t>
-  </si>
-  <si>
-    <t>https://identifiers.org/RRID:SCR_023732</t>
-  </si>
-  <si>
     <t>metadata_schema_id</t>
   </si>
   <si>
@@ -638,7 +495,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-11-01T13:54:36-07:00</t>
+    <t>2023-11-01T15:37:30-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -697,7 +554,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyAlignment="true" applyFill="true">
       <alignment horizontal="center"/>
@@ -719,8 +576,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -731,7 +586,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -753,9 +608,7 @@
     <col min="14" max="14" style="15" width="15.05859375" customWidth="true" bestFit="true"/>
     <col min="15" max="15" style="16" width="26.43359375" customWidth="true" bestFit="true"/>
     <col min="16" max="16" style="17" width="25.2734375" customWidth="true" bestFit="true"/>
-    <col min="17" max="17" style="18" width="29.08203125" customWidth="true" bestFit="true"/>
-    <col min="18" max="18" style="19" width="28.48828125" customWidth="true" bestFit="true"/>
-    <col min="19" max="19" style="20" width="19.61328125" customWidth="true" bestFit="true"/>
+    <col min="17" max="17" style="18" width="19.61328125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -810,20 +663,14 @@
       <c r="Q1" t="s" s="1">
         <v>108</v>
       </c>
-      <c r="R1" t="s" s="1">
-        <v>123</v>
-      </c>
-      <c r="S1" t="s" s="1">
-        <v>150</v>
-      </c>
     </row>
     <row r="2">
-      <c r="S2" t="s">
-        <v>151</v>
+      <c r="Q2" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="13">
+  <dataValidations count="11">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'dataset_type'!$A$1:$A$36</formula1>
     </dataValidation>
@@ -862,63 +709,10 @@
     <dataValidation type="list" sqref="P2:P1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'permeabilization_time_unit'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="Q2:Q1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_vendor'!$A$1:$A$7</formula1>
-    </dataValidation>
-    <dataValidation type="list" sqref="R2:R1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_model'!$A$1:$A$14</formula1>
-    </dataValidation>
   </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="11.83203125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.1875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="27.9921875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="80.6640625" customWidth="true" bestFit="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C2" t="s">
-        <v>156</v>
-      </c>
-      <c r="D2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -1398,191 +1192,44 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.1875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="27.9921875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="80.6640625" customWidth="true" bestFit="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B1" t="s">
-        <v>110</v>
+        <v>111</v>
+      </c>
+      <c r="C1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="D2" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>121</v>
-      </c>
-      <c r="B7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>132</v>
-      </c>
-      <c r="B6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>134</v>
-      </c>
-      <c r="B7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>136</v>
-      </c>
-      <c r="B8" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>138</v>
-      </c>
-      <c r="B9" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>140</v>
-      </c>
-      <c r="B10" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>142</v>
-      </c>
-      <c r="B11" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>144</v>
-      </c>
-      <c r="B12" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>146</v>
-      </c>
-      <c r="B13" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>148</v>
-      </c>
-      <c r="B14" t="s">
-        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Visium v2.0 to use old dataset type branch
</commit_message>
<xml_diff>
--- a/visium/latest/visium.xlsx
+++ b/visium/latest/visium.xlsx
@@ -151,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="113">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -249,12 +249,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000202</t>
   </si>
   <si>
-    <t>RNAseq (Visium)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000188</t>
-  </si>
-  <si>
     <t>Cell DIVE</t>
   </si>
   <si>
@@ -267,6 +261,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000160</t>
   </si>
   <si>
+    <t>GeoMx (NGS)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000300</t>
+  </si>
+  <si>
     <t>CyCIF</t>
   </si>
   <si>
@@ -279,12 +279,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
   </si>
   <si>
-    <t>GeoMx</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000216</t>
-  </si>
-  <si>
     <t>RNAseq (bulk)</t>
   </si>
   <si>
@@ -303,12 +297,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000296</t>
   </si>
   <si>
-    <t>RNAseq (GeoMx)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000214</t>
-  </si>
-  <si>
     <t>Histology</t>
   </si>
   <si>
@@ -345,6 +333,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
   </si>
   <si>
+    <t>GeoMx (nCounter)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000301</t>
+  </si>
+  <si>
     <t>PhenoCycler</t>
   </si>
   <si>
@@ -489,7 +483,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-11-07T20:06:36-08:00</t>
+    <t>2023-11-15T17:24:29-08:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -619,54 +613,54 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
+        <v>72</v>
+      </c>
+      <c r="F1" t="s" s="1">
+        <v>73</v>
+      </c>
+      <c r="G1" t="s" s="1">
         <v>74</v>
       </c>
-      <c r="F1" t="s" s="1">
+      <c r="H1" t="s" s="1">
         <v>75</v>
       </c>
-      <c r="G1" t="s" s="1">
-        <v>76</v>
-      </c>
-      <c r="H1" t="s" s="1">
-        <v>77</v>
-      </c>
       <c r="I1" t="s" s="1">
+        <v>80</v>
+      </c>
+      <c r="J1" t="s" s="1">
+        <v>81</v>
+      </c>
+      <c r="K1" t="s" s="1">
         <v>82</v>
       </c>
-      <c r="J1" t="s" s="1">
+      <c r="L1" t="s" s="1">
         <v>83</v>
       </c>
-      <c r="K1" t="s" s="1">
+      <c r="M1" t="s" s="1">
         <v>84</v>
       </c>
-      <c r="L1" t="s" s="1">
-        <v>85</v>
-      </c>
-      <c r="M1" t="s" s="1">
-        <v>86</v>
-      </c>
       <c r="N1" t="s" s="1">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2">
       <c r="Q2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="11">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$35</formula1>
+      <formula1>'dataset_type'!$A$1:$A$34</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="between" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be a number" showErrorMessage="true">
       <formula1>-3.4028235E38</formula1>
@@ -712,7 +706,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -988,14 +982,6 @@
       </c>
       <c r="B34" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s">
-        <v>72</v>
-      </c>
-      <c r="B35" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1013,18 +999,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1042,18 +1028,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1071,10 +1057,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1092,62 +1078,62 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1165,10 +1151,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1192,30 +1178,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" t="s">
         <v>109</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>111</v>
-      </c>
-      <c r="D1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" t="s">
         <v>110</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>112</v>
-      </c>
-      <c r="D2" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>